<commit_message>
update datasets and corresponding models
</commit_message>
<xml_diff>
--- a/results对比.xlsx
+++ b/results对比.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_________________________PythonProject\ST-EVCDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB8887A-2699-4344-8BFC-1C21D07ADB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FA7EBF-BBB8-432E-AD89-3ED035648176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="zone42" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
-    <sheet name="30min" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId1"/>
+    <sheet name="zone42" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="30min" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="53">
   <si>
     <t>RMSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -215,6 +216,22 @@
   </si>
   <si>
     <t>all zones</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LSTM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChatEV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prelen=6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -290,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -306,6 +323,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1535,11 +1555,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0A8D63-949F-416F-80F6-D42117F8D6D1}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2.0601336024022401E-3</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4.5388694654090303E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.14729538904564601</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.71040896052998104</v>
+      </c>
+      <c r="F2" s="7">
+        <v>3.7178800653496498E-2</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.41792575803604798</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3.65541949868202E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4.6053074300289099E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>13.724164009094199</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.69853866100311202</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3.65541949868202E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.40059769153594899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1.6644386142622199E-3</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4.07975319628801E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.115288144526433</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.60691025360126605</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3.1762261720870003E-2</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.52972620631860801</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3DAF-3846-47F5-A121-0221C6ACF96F}">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2372,20 +2500,112 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87309E1E-6F11-4CCE-838D-E40BBB73FB75}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.4681726000000001E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.12116817100000001</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.39348560700000001</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.95338167799999995</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.10298618399999999</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.14422713700000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="4">
+        <v>6.5392410000000003E-3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8.0865571999999997E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.33622685299999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.55253380500000004</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5.9685799999999997E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.61883875600000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3.65541949868202E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4.6053074300289099E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>13.724164009094199</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.69853866100311202</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3.65541949868202E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.40059769153594899</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I42"/>
   <sheetViews>

</xml_diff>